<commit_message>
added code in master
</commit_message>
<xml_diff>
--- a/RestAssuredAutomation2/Test Excel Files/CitiesData.xlsx
+++ b/RestAssuredAutomation2/Test Excel Files/CitiesData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PositiveTestCasesData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="17">
   <si>
     <t>CityName</t>
   </si>
@@ -55,19 +55,22 @@
     <t>Noida</t>
   </si>
   <si>
+    <t>TC_01_Verify Chandigarh City Info</t>
+  </si>
+  <si>
+    <t>TC_02_Verify Delhi City Info</t>
+  </si>
+  <si>
+    <t>TC_03_Verify Noid City Info</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>TC_01_Verify Chandigarh City Info</t>
-  </si>
-  <si>
-    <t>TC_02_Verify Delhi City Info</t>
-  </si>
-  <si>
-    <t>TC_03_Verify Noid City Info</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -437,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +476,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -488,12 +491,12 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -508,12 +511,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -528,7 +531,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -539,12 +542,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>200</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>200</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>